<commit_message>
Into the Results section - also broke off introduction into two sections
</commit_message>
<xml_diff>
--- a/coling2016/props/Dataset-stats-COLING-2016.xlsx
+++ b/coling2016/props/Dataset-stats-COLING-2016.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="27700" windowHeight="15840" tabRatio="630"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="27700" windowHeight="15840" tabRatio="630" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SliceDatasetStats" sheetId="15" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="115">
   <si>
     <t>Baby Products</t>
   </si>
@@ -358,6 +358,15 @@
   </si>
   <si>
     <t>Business Unit 2</t>
+  </si>
+  <si>
+    <t>ln=9.26966925683351</t>
+  </si>
+  <si>
+    <t>ln=6.017081357148303</t>
+  </si>
+  <si>
+    <t>ln=11.53770663030109</t>
   </si>
 </sst>
 </file>
@@ -424,7 +433,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="574">
+  <cellStyleXfs count="576">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -521,6 +530,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1007,7 +1018,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="574">
+  <cellStyles count="576">
     <cellStyle name="Comma 2" xfId="95"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1295,6 +1306,7 @@
     <cellStyle name="Followed Hyperlink" xfId="569" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="571" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="573" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="575" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1581,6 +1593,7 @@
     <cellStyle name="Hyperlink" xfId="568" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="570" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="572" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="574" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1804,11 +1817,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1991644712"/>
-        <c:axId val="-2076158088"/>
+        <c:axId val="-2125541912"/>
+        <c:axId val="-2052041640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1991644712"/>
+        <c:axId val="-2125541912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1837,7 +1850,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2076158088"/>
+        <c:crossAx val="-2052041640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1845,7 +1858,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2076158088"/>
+        <c:axId val="-2052041640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6.0"/>
@@ -1867,7 +1880,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1991644712"/>
+        <c:crossAx val="-2125541912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2080,11 +2093,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2077363704"/>
-        <c:axId val="-1992230040"/>
+        <c:axId val="-2051613128"/>
+        <c:axId val="-2051610008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2077363704"/>
+        <c:axId val="-2051613128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2113,7 +2126,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1992230040"/>
+        <c:crossAx val="-2051610008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2121,7 +2134,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1992230040"/>
+        <c:axId val="-2051610008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="260.0"/>
@@ -2144,7 +2157,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2077363704"/>
+        <c:crossAx val="-2051613128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="50.0"/>
@@ -2411,11 +2424,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2076069208"/>
-        <c:axId val="-2050436648"/>
+        <c:axId val="-2125545704"/>
+        <c:axId val="-2125853864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2076069208"/>
+        <c:axId val="-2125545704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2444,7 +2457,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2050436648"/>
+        <c:crossAx val="-2125853864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2452,7 +2465,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2050436648"/>
+        <c:axId val="-2125853864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2473,7 +2486,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2076069208"/>
+        <c:crossAx val="-2125545704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2732,11 +2745,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2075671928"/>
-        <c:axId val="-2011836904"/>
+        <c:axId val="-2051704232"/>
+        <c:axId val="-2051748312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2075671928"/>
+        <c:axId val="-2051704232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2765,7 +2778,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2011836904"/>
+        <c:crossAx val="-2051748312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2773,7 +2786,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2011836904"/>
+        <c:axId val="-2051748312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2600.0"/>
@@ -2796,7 +2809,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2075671928"/>
+        <c:crossAx val="-2051704232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3002,11 +3015,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2080086872"/>
-        <c:axId val="-2055169128"/>
+        <c:axId val="-2051944696"/>
+        <c:axId val="-2051670136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2080086872"/>
+        <c:axId val="-2051944696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3035,7 +3048,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2055169128"/>
+        <c:crossAx val="-2051670136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3043,7 +3056,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2055169128"/>
+        <c:axId val="-2051670136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6.0"/>
@@ -3065,7 +3078,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2080086872"/>
+        <c:crossAx val="-2051944696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3272,11 +3285,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2051676584"/>
-        <c:axId val="-2125501656"/>
+        <c:axId val="-2079435272"/>
+        <c:axId val="-2051554296"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2051676584"/>
+        <c:axId val="-2079435272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3305,7 +3318,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2125501656"/>
+        <c:crossAx val="-2051554296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3313,7 +3326,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2125501656"/>
+        <c:axId val="-2051554296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="260.0"/>
@@ -3336,7 +3349,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2051676584"/>
+        <c:crossAx val="-2079435272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3884,8 +3897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4453,6 +4466,9 @@
         <f>PEARSON(D3:D18,E3:E18)</f>
         <v>0.64286470540130303</v>
       </c>
+      <c r="F19" t="s">
+        <v>112</v>
+      </c>
       <c r="O19" s="1" t="s">
         <v>31</v>
       </c>
@@ -4473,6 +4489,10 @@
       <c r="E20">
         <f>SUM(E3:E18)</f>
         <v>12160483</v>
+      </c>
+      <c r="F20">
+        <f>LOG($E$20/$D$20)</f>
+        <v>4.0257662073110119</v>
       </c>
     </row>
     <row r="21" spans="1:18">
@@ -4869,7 +4889,7 @@
   <dimension ref="A1:T56"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P40" sqref="P40"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5781,6 +5801,9 @@
         <f>PEARSON(E2:E26,F2:F26)</f>
         <v>0.26906993846390143</v>
       </c>
+      <c r="G27" t="s">
+        <v>113</v>
+      </c>
       <c r="P27">
         <v>790000</v>
       </c>
@@ -5810,8 +5833,8 @@
         <v>7463975</v>
       </c>
       <c r="G28">
-        <f>AVERAGE(F2:F26)</f>
-        <v>298559</v>
+        <f>LOG10($F$28/$E$28)</f>
+        <v>2.6131852305724372</v>
       </c>
       <c r="Q28" s="1" t="s">
         <v>31</v>
@@ -6281,8 +6304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6793,6 +6816,9 @@
       <c r="E17">
         <v>2672169</v>
       </c>
+      <c r="F17" t="s">
+        <v>114</v>
+      </c>
       <c r="M17">
         <v>260000</v>
       </c>
@@ -6821,6 +6847,10 @@
       <c r="E18">
         <f>SUM(E3:E17)</f>
         <v>58532683</v>
+      </c>
+      <c r="F18">
+        <f>LOG10($E$18/$D$18)</f>
+        <v>5.0107623233583247</v>
       </c>
       <c r="N18" t="s">
         <v>31</v>

</xml_diff>